<commit_message>
Refine Excel template hierarchy and leaf fields
</commit_message>
<xml_diff>
--- a/artifacts/Chronoplan_Template.xlsx
+++ b/artifacts/Chronoplan_Template.xlsx
@@ -430,7 +430,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -451,20 +451,25 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
+          <t>Activity Status</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
           <t>BL Project Finish</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>Finish</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>Units % Complete</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>Variance - BL Project Finish Date</t>
         </is>
@@ -477,16 +482,17 @@
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
-      <c r="C2" s="2" t="n">
+      <c r="C2" t="inlineStr"/>
+      <c r="D2" s="2" t="n">
         <v>46069</v>
       </c>
-      <c r="D2" s="2" t="n">
+      <c r="E2" s="2" t="n">
         <v>46076</v>
       </c>
-      <c r="E2" t="n">
+      <c r="F2" t="n">
         <v>85</v>
       </c>
-      <c r="F2" t="n">
+      <c r="G2" t="n">
         <v>-1</v>
       </c>
     </row>
@@ -497,16 +503,17 @@
         </is>
       </c>
       <c r="B3" t="inlineStr"/>
-      <c r="C3" s="2" t="n">
+      <c r="C3" t="inlineStr"/>
+      <c r="D3" s="2" t="n">
         <v>46055</v>
       </c>
-      <c r="D3" s="2" t="n">
+      <c r="E3" s="2" t="n">
         <v>46062</v>
       </c>
-      <c r="E3" t="n">
+      <c r="F3" t="n">
         <v>82</v>
       </c>
-      <c r="F3" t="n">
+      <c r="G3" t="n">
         <v>-1</v>
       </c>
     </row>
@@ -521,16 +528,21 @@
           <t>Mobilize crew</t>
         </is>
       </c>
-      <c r="C4" s="2" t="n">
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Completed</t>
+        </is>
+      </c>
+      <c r="D4" s="2" t="n">
         <v>46041</v>
       </c>
-      <c r="D4" s="2" t="n">
+      <c r="E4" s="2" t="n">
         <v>46048</v>
       </c>
-      <c r="E4" t="n">
+      <c r="F4" t="n">
         <v>95</v>
       </c>
-      <c r="F4" t="n">
+      <c r="G4" t="n">
         <v>1</v>
       </c>
     </row>
@@ -545,16 +557,21 @@
           <t>Temporary works</t>
         </is>
       </c>
-      <c r="C5" s="2" t="n">
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>In Progress</t>
+        </is>
+      </c>
+      <c r="D5" s="2" t="n">
         <v>46048</v>
       </c>
-      <c r="D5" s="2" t="n">
+      <c r="E5" s="2" t="n">
         <v>46055</v>
       </c>
-      <c r="E5" t="n">
+      <c r="F5" t="n">
         <v>72</v>
       </c>
-      <c r="F5" t="n">
+      <c r="G5" t="n">
         <v>2</v>
       </c>
     </row>
@@ -569,16 +586,21 @@
           <t>Foundations</t>
         </is>
       </c>
-      <c r="C6" s="2" t="n">
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Not Started</t>
+        </is>
+      </c>
+      <c r="D6" s="2" t="n">
         <v>46055</v>
       </c>
-      <c r="D6" s="2" t="n">
+      <c r="E6" s="2" t="n">
         <v>46062</v>
       </c>
-      <c r="E6" t="n">
+      <c r="F6" t="n">
         <v>61</v>
       </c>
-      <c r="F6" t="n">
+      <c r="G6" t="n">
         <v>3</v>
       </c>
     </row>
@@ -706,7 +728,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>A-110</t>
+          <t xml:space="preserve">  A-110</t>
         </is>
       </c>
       <c r="B3" s="2" t="n">
@@ -754,7 +776,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>A-111</t>
+          <t xml:space="preserve">    A-111</t>
         </is>
       </c>
       <c r="B4" s="2" t="n">
@@ -802,7 +824,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>A-112</t>
+          <t xml:space="preserve">    A-112</t>
         </is>
       </c>
       <c r="B5" s="2" t="n">
@@ -850,7 +872,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>A-120</t>
+          <t xml:space="preserve">  A-120</t>
         </is>
       </c>
       <c r="B6" s="2" t="n">
@@ -1019,7 +1041,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>A-110</t>
+          <t xml:space="preserve">  A-110</t>
         </is>
       </c>
       <c r="B3" s="2" t="n">
@@ -1067,7 +1089,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>A-111</t>
+          <t xml:space="preserve">    A-111</t>
         </is>
       </c>
       <c r="B4" s="2" t="n">
@@ -1115,7 +1137,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>A-112</t>
+          <t xml:space="preserve">    A-112</t>
         </is>
       </c>
       <c r="B5" s="2" t="n">
@@ -1163,7 +1185,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>A-120</t>
+          <t xml:space="preserve">  A-120</t>
         </is>
       </c>
       <c r="B6" s="2" t="n">
@@ -1332,7 +1354,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>A-110</t>
+          <t xml:space="preserve">  A-110</t>
         </is>
       </c>
       <c r="B3" s="2" t="n">
@@ -1380,7 +1402,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>A-111</t>
+          <t xml:space="preserve">    A-111</t>
         </is>
       </c>
       <c r="B4" s="2" t="n">
@@ -1428,7 +1450,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>A-112</t>
+          <t xml:space="preserve">    A-112</t>
         </is>
       </c>
       <c r="B5" s="2" t="n">
@@ -1476,7 +1498,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>A-120</t>
+          <t xml:space="preserve">  A-120</t>
         </is>
       </c>
       <c r="B6" s="2" t="n">
@@ -1532,7 +1554,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A13"/>
+  <dimension ref="A1:A15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1540,7 +1562,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="80" customWidth="1" min="1" max="1"/>
+    <col width="90" customWidth="1" min="1" max="1"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1577,50 +1599,64 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>- Activity Name is required for leaf activities (last children).</t>
+          <t>- Activity Name is required only for leaf activities.</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
+          <t>- Activity Status must be filled when Activity Name is filled.</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
           <t>- Dates can be Excel dates or YYYY-MM-DD.</t>
         </is>
       </c>
     </row>
-    <row r="8">
-      <c r="A8" t="inlineStr"/>
-    </row>
     <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>Resource Assignments sheets:</t>
-        </is>
-      </c>
+      <c r="A9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>- Keep one table per sheet with the same Activity IDs.</t>
+          <t>Resource Assignments sheets:</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>- Spreadsheet Field must be one of:</t>
+          <t>- Keep one table per sheet with the same Activity IDs.</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t xml:space="preserve">  Cum Budgeted Units, Cum Actual Units, Cum Remaining Early Units.</t>
+          <t>- Keep the same indentation in Activity ID for all tables.</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
+        <is>
+          <t>- Spreadsheet Field must be one of:</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  Cum Budgeted Units, Cum Actual Units, Cum Remaining Early Units.</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
         <is>
           <t>- Weekly columns are week start dates (Monday).</t>
         </is>

</xml_diff>

<commit_message>
Add Budgeted Labor Units to template and docs
</commit_message>
<xml_diff>
--- a/artifacts/Chronoplan_Template.xlsx
+++ b/artifacts/Chronoplan_Template.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Activities" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Ressource Assign. Budgeted" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Ressource Assign. Actual" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Ressource Assign. Remaining" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="README" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="Activities" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Ressource Assign. Budgeted" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Ressource Assign. Actual" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Ressource Assign. Remaining" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="README" sheetId="5" state="visible" r:id="rId5"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -430,7 +430,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -474,6 +474,11 @@
           <t>Variance - BL Project Finish Date</t>
         </is>
       </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>Budgeted Labor Units</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -481,8 +486,6 @@
           <t>A-100</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr"/>
-      <c r="C2" t="inlineStr"/>
       <c r="D2" s="2" t="n">
         <v>46069</v>
       </c>
@@ -495,6 +498,9 @@
       <c r="G2" t="n">
         <v>-1</v>
       </c>
+      <c r="H2" t="n">
+        <v>1000</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -502,8 +508,6 @@
           <t xml:space="preserve">  A-110</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr"/>
-      <c r="C3" t="inlineStr"/>
       <c r="D3" s="2" t="n">
         <v>46055</v>
       </c>
@@ -516,6 +520,9 @@
       <c r="G3" t="n">
         <v>-1</v>
       </c>
+      <c r="H3" t="n">
+        <v>600</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -545,6 +552,9 @@
       <c r="G4" t="n">
         <v>1</v>
       </c>
+      <c r="H4" t="n">
+        <v>300</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -574,6 +584,9 @@
       <c r="G5" t="n">
         <v>2</v>
       </c>
+      <c r="H5" t="n">
+        <v>300</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -602,6 +615,9 @@
       </c>
       <c r="G6" t="n">
         <v>3</v>
+      </c>
+      <c r="H6" t="n">
+        <v>400</v>
       </c>
     </row>
   </sheetData>
@@ -1554,7 +1570,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A15"/>
+  <dimension ref="A1:A31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1572,9 +1588,7 @@
         </is>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="inlineStr"/>
-    </row>
+    <row r="2"/>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
@@ -1585,83 +1599,103 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>- Keep one header row with the required columns.</t>
+          <t>- Include Budgeted Labor Units (last column) for all activities.</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>- Indent Activity ID with spaces to represent the hierarchy.</t>
+          <t>- Keep one header row with the required columns.</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>- Activity Name is required only for leaf activities.</t>
+          <t>- Indent Activity ID with spaces to represent the hierarchy.</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>- Activity Status must be filled when Activity Name is filled.</t>
+          <t>- Activity Name is required only for leaf activities.</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
+          <t>- Activity Status must be filled when Activity Name is filled.</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
           <t>- Dates can be Excel dates or YYYY-MM-DD.</t>
         </is>
       </c>
     </row>
-    <row r="9">
-      <c r="A9" t="inlineStr"/>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>Resource Assignments sheets:</t>
-        </is>
-      </c>
-    </row>
+    <row r="10"/>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>- Keep one table per sheet with the same Activity IDs.</t>
+          <t>Resource Assignments sheets:</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>- Keep the same indentation in Activity ID for all tables.</t>
+          <t>- Keep one table per sheet with the same Activity IDs.</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>- Spreadsheet Field must be one of:</t>
+          <t>- Keep the same indentation in Activity ID for all tables.</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t xml:space="preserve">  Cum Budgeted Units, Cum Actual Units, Cum Remaining Early Units.</t>
+          <t>- Spreadsheet Field must be one of:</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
+          <t xml:space="preserve">  Cum Budgeted Units, Cum Actual Units, Cum Remaining Early Units.</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
           <t>- Weekly columns are week start dates (Monday).</t>
         </is>
       </c>
     </row>
+    <row r="17"/>
+    <row r="18"/>
+    <row r="19"/>
+    <row r="20"/>
+    <row r="21"/>
+    <row r="22"/>
+    <row r="23"/>
+    <row r="24"/>
+    <row r="25"/>
+    <row r="26"/>
+    <row r="27"/>
+    <row r="28"/>
+    <row r="29"/>
+    <row r="30"/>
+    <row r="31"/>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>